<commit_message>
Correccion de lectura a data
</commit_message>
<xml_diff>
--- a/data/Siniestros.xlsx
+++ b/data/Siniestros.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafae\Curso Data Frames\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dc947767ebb0dc92/Documentos/GitHub/WorkShopDS/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A8BC48-C636-4883-A568-7D5A465C79CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{1F71FF50-7A3A-4DC5-BB5B-EDD74F48D0EE}"/>
+    <workbookView xWindow="936" yWindow="2208" windowWidth="17256" windowHeight="8892" activeTab="1" xr2:uid="{1F71FF50-7A3A-4DC5-BB5B-EDD74F48D0EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Siniestros" sheetId="1" r:id="rId1"/>

</xml_diff>